<commit_message>
aplicacao indice ate 13-10-2020
</commit_message>
<xml_diff>
--- a/low-flow-index/dados-saida/uniao_da_vitoria.xlsx
+++ b/low-flow-index/dados-saida/uniao_da_vitoria.xlsx
@@ -394,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,10 +437,10 @@
         <v>29</v>
       </c>
       <c r="F2">
-        <v>0.4482206389619964</v>
+        <v>0.4529604389419829</v>
       </c>
       <c r="G2">
-        <v>0.4744987743216194</v>
+        <v>0.5753401078409786</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -460,10 +460,10 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>0.120769776985929</v>
+        <v>0.1177228730614828</v>
       </c>
       <c r="G3">
-        <v>0.2133914065945986</v>
+        <v>0.2848734791496697</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -483,10 +483,10 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>0.05392769858394352</v>
+        <v>0.04884285606111181</v>
       </c>
       <c r="G4">
-        <v>0.1337547339382184</v>
+        <v>0.1829027603585654</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -506,10 +506,10 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>0.04492663651297382</v>
+        <v>0.03955750888195161</v>
       </c>
       <c r="G5">
-        <v>0.1204314655676566</v>
+        <v>0.1645731726633032</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -523,16 +523,16 @@
         <v>12316</v>
       </c>
       <c r="D6">
-        <v>48.5889</v>
+        <v>52.38890000000001</v>
       </c>
       <c r="E6" s="3">
         <v>41</v>
       </c>
       <c r="F6">
-        <v>0.07371911617506027</v>
+        <v>0.07770909347237369</v>
       </c>
       <c r="G6">
-        <v>0.1601712955579285</v>
+        <v>0.230950582805072</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -552,1275 +552,1298 @@
         <v>25</v>
       </c>
       <c r="F7">
-        <v>0.4465129360861875</v>
+        <v>0.4512234141186302</v>
       </c>
       <c r="G7">
-        <v>0.4733112161827278</v>
+        <v>0.5741248761263826</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
-        <v>12733</v>
+        <v>12666</v>
       </c>
       <c r="C8" s="2">
-        <v>12750</v>
+        <v>12671</v>
       </c>
       <c r="D8">
-        <v>332.4859999999999</v>
+        <v>19.13379999999997</v>
       </c>
       <c r="E8" s="3">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>0.5235213937847013</v>
+        <v>0.001006048557626691</v>
       </c>
       <c r="G8">
-        <v>0.5264547322673958</v>
+        <v>0.02641836371270655</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>12912</v>
+        <v>12733</v>
       </c>
       <c r="C9" s="2">
-        <v>12945</v>
+        <v>12750</v>
       </c>
       <c r="D9">
-        <v>216.3121999999999</v>
+        <v>332.4859999999999</v>
       </c>
       <c r="E9" s="3">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F9">
-        <v>0.3745648047982461</v>
+        <v>0.5294090397474582</v>
       </c>
       <c r="G9">
-        <v>0.422573297744201</v>
+        <v>0.6276488308994788</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
-        <v>14692</v>
+        <v>12912</v>
       </c>
       <c r="C10" s="2">
-        <v>14698</v>
+        <v>12945</v>
       </c>
       <c r="D10">
-        <v>66.07299999999999</v>
+        <v>216.3121999999999</v>
       </c>
       <c r="E10" s="3">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="F10">
-        <v>0.1108749356863682</v>
+        <v>0.377918467881278</v>
       </c>
       <c r="G10">
-        <v>0.2029957927523801</v>
+        <v>0.5213806288392363</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2">
-        <v>15653</v>
+        <v>14692</v>
       </c>
       <c r="C11" s="2">
-        <v>15660</v>
+        <v>14698</v>
       </c>
       <c r="D11">
-        <v>41.86799999999998</v>
+        <v>66.07299999999999</v>
       </c>
       <c r="E11" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11">
-        <v>0.0590267289371721</v>
+        <v>0.1075346739753989</v>
       </c>
       <c r="G11">
-        <v>0.1408941099812947</v>
+        <v>0.2721042111986424</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2">
-        <v>15713</v>
+        <v>15653</v>
       </c>
       <c r="C12" s="2">
-        <v>15724</v>
+        <v>15660</v>
       </c>
       <c r="D12">
-        <v>31.38399999999999</v>
+        <v>41.86799999999998</v>
       </c>
       <c r="E12" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F12">
-        <v>0.03564124664008766</v>
+        <v>0.05410191626796727</v>
       </c>
       <c r="G12">
-        <v>0.1054607685001308</v>
+        <v>0.1925257988762217</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
-        <v>15806</v>
+        <v>15713</v>
       </c>
       <c r="C13" s="2">
-        <v>15811</v>
+        <v>15724</v>
       </c>
       <c r="D13">
-        <v>22.571</v>
+        <v>31.38399999999999</v>
       </c>
       <c r="E13" s="3">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F13">
-        <v>0.01553404668422644</v>
+        <v>0.02997647482037862</v>
       </c>
       <c r="G13">
-        <v>0.0656258276119713</v>
+        <v>0.1432606226521859</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2">
-        <v>15835</v>
+        <v>15806</v>
       </c>
       <c r="C14" s="2">
-        <v>15848</v>
+        <v>15811</v>
       </c>
       <c r="D14">
-        <v>112.1524</v>
+        <v>22.571</v>
       </c>
       <c r="E14" s="3">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F14">
-        <v>0.2018141808365812</v>
+        <v>0.009220893268835482</v>
       </c>
       <c r="G14">
-        <v>0.289049360180847</v>
+        <v>0.07957250513004152</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2">
-        <v>16224</v>
+        <v>15835</v>
       </c>
       <c r="C15" s="2">
-        <v>16313</v>
+        <v>15848</v>
       </c>
       <c r="D15">
-        <v>1241.5981</v>
+        <v>112.1524</v>
       </c>
       <c r="E15" s="3">
-        <v>90</v>
+        <v>14</v>
       </c>
       <c r="F15">
-        <v>0.9433038680638326</v>
+        <v>0.2010550213662789</v>
       </c>
       <c r="G15">
-        <v>0.8637567154464959</v>
+        <v>0.374426565246658</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
-        <v>16337</v>
+        <v>16224</v>
       </c>
       <c r="C16" s="2">
-        <v>16383</v>
+        <v>16313</v>
       </c>
       <c r="D16">
-        <v>752.0580999999996</v>
+        <v>1242.6881</v>
       </c>
       <c r="E16" s="3">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="F16">
-        <v>0.8216085108107501</v>
+        <v>0.9471514783503885</v>
       </c>
       <c r="G16">
-        <v>0.7432144387471261</v>
+        <v>0.9213306635642655</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
-        <v>16440</v>
+        <v>16337</v>
       </c>
       <c r="C17" s="2">
-        <v>16485</v>
+        <v>16383</v>
       </c>
       <c r="D17">
-        <v>837.2021999999999</v>
+        <v>730.4280999999996</v>
       </c>
       <c r="E17" s="3">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F17">
-        <v>0.8538530367712394</v>
+        <v>0.8190860946412644</v>
       </c>
       <c r="G17">
-        <v>0.7709439975651277</v>
+        <v>0.8203442147426415</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B18" s="2">
-        <v>17893</v>
+        <v>16440</v>
       </c>
       <c r="C18" s="2">
-        <v>17906</v>
+        <v>16485</v>
       </c>
       <c r="D18">
-        <v>204.8097</v>
+        <v>837.2021999999999</v>
       </c>
       <c r="E18" s="3">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="F18">
-        <v>0.3574907497963437</v>
+        <v>0.8600171293204313</v>
       </c>
       <c r="G18">
-        <v>0.4102659839436698</v>
+        <v>0.8497593115723698</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="2">
-        <v>17926</v>
+        <v>17893</v>
       </c>
       <c r="C19" s="2">
-        <v>17962</v>
+        <v>17906</v>
       </c>
       <c r="D19">
-        <v>804.2808999999997</v>
+        <v>204.8097</v>
       </c>
       <c r="E19" s="3">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="F19">
-        <v>0.842141501266091</v>
+        <v>0.3604892821217764</v>
       </c>
       <c r="G19">
-        <v>0.7606581842317413</v>
+        <v>0.5083413410509233</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B20" s="2">
-        <v>18201</v>
+        <v>17926</v>
       </c>
       <c r="C20" s="2">
-        <v>18260</v>
+        <v>17962</v>
       </c>
       <c r="D20">
-        <v>370.9396999999999</v>
+        <v>804.2808999999997</v>
       </c>
       <c r="E20" s="3">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="F20">
-        <v>0.5645490413184637</v>
+        <v>0.8484968805086426</v>
       </c>
       <c r="G20">
-        <v>0.5546473346244187</v>
+        <v>0.8413208553348218</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2">
-        <v>18853</v>
+        <v>18201</v>
       </c>
       <c r="C21" s="2">
-        <v>18915</v>
+        <v>18260</v>
       </c>
       <c r="D21">
-        <v>1377.7569</v>
+        <v>370.9396999999999</v>
       </c>
       <c r="E21" s="3">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F21">
-        <v>0.9587815678987917</v>
+        <v>0.5709331452572712</v>
       </c>
       <c r="G21">
-        <v>0.884909002514932</v>
+        <v>0.6553280378850799</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B22" s="2">
-        <v>19050</v>
+        <v>18853</v>
       </c>
       <c r="C22" s="2">
-        <v>19071</v>
+        <v>18915</v>
       </c>
       <c r="D22">
-        <v>107.963</v>
+        <v>1363.2869</v>
       </c>
       <c r="E22" s="3">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F22">
-        <v>0.1939457493679151</v>
+        <v>0.9604439854788251</v>
       </c>
       <c r="G22">
-        <v>0.2822584712183672</v>
+        <v>0.9346513613764266</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="2">
-        <v>19093</v>
+        <v>19050</v>
       </c>
       <c r="C23" s="2">
-        <v>19149</v>
+        <v>19071</v>
       </c>
       <c r="D23">
-        <v>834.8418999999997</v>
+        <v>107.963</v>
       </c>
       <c r="E23" s="3">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="F23">
-        <v>0.8530430869309424</v>
+        <v>0.1929737554386703</v>
       </c>
       <c r="G23">
-        <v>0.7702238519322977</v>
+        <v>0.3666017075283696</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2">
-        <v>20119</v>
+        <v>19093</v>
       </c>
       <c r="C24" s="2">
-        <v>20144</v>
+        <v>19149</v>
       </c>
       <c r="D24">
-        <v>51.249</v>
+        <v>834.8418999999997</v>
       </c>
       <c r="E24" s="3">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="F24">
-        <v>0.07947072412426731</v>
+        <v>0.8592211580326078</v>
       </c>
       <c r="G24">
-        <v>0.1672849148161984</v>
+        <v>0.8491715539014487</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B25" s="2">
-        <v>20778</v>
+        <v>20119</v>
       </c>
       <c r="C25" s="2">
-        <v>20796</v>
+        <v>20144</v>
       </c>
       <c r="D25">
-        <v>300.3779</v>
+        <v>51.249</v>
       </c>
       <c r="E25" s="3">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F25">
-        <v>0.4863176747318962</v>
+        <v>0.0751800696806284</v>
       </c>
       <c r="G25">
-        <v>0.5008625505274135</v>
+        <v>0.2271351965703581</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2">
-        <v>21855</v>
+        <v>20778</v>
       </c>
       <c r="C26" s="2">
-        <v>21924</v>
+        <v>20796</v>
       </c>
       <c r="D26">
-        <v>938.6927999999998</v>
+        <v>300.3779</v>
       </c>
       <c r="E26" s="3">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="F26">
-        <v>0.8847655177473782</v>
+        <v>0.4916745529134886</v>
       </c>
       <c r="G26">
-        <v>0.7995894043827591</v>
+        <v>0.6020925612849669</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B27" s="2">
-        <v>21941</v>
+        <v>21855</v>
       </c>
       <c r="C27" s="2">
-        <v>21959</v>
+        <v>21924</v>
       </c>
       <c r="D27">
-        <v>87.87499999999996</v>
+        <v>938.6927999999998</v>
       </c>
       <c r="E27" s="3">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="F27">
-        <v>0.1551257645716873</v>
+        <v>0.8903041747537608</v>
       </c>
       <c r="G27">
-        <v>0.2472097767294026</v>
+        <v>0.8727518760646145</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B28" s="2">
-        <v>23008</v>
+        <v>21941</v>
       </c>
       <c r="C28" s="2">
-        <v>23021</v>
+        <v>21959</v>
       </c>
       <c r="D28">
-        <v>123.4271</v>
+        <v>87.87499999999996</v>
       </c>
       <c r="E28" s="3">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F28">
-        <v>0.2226106383920583</v>
+        <v>0.1530741280505891</v>
       </c>
       <c r="G28">
-        <v>0.3065805231491364</v>
+        <v>0.3255814890873994</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B29" s="2">
-        <v>23173</v>
+        <v>23008</v>
       </c>
       <c r="C29" s="2">
-        <v>23281</v>
+        <v>23021</v>
       </c>
       <c r="D29">
-        <v>1702.3454</v>
+        <v>123.4271</v>
       </c>
       <c r="E29" s="3">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="F29">
-        <v>0.9807241975790428</v>
+        <v>0.2224040040683128</v>
       </c>
       <c r="G29">
-        <v>0.9223585387953226</v>
+        <v>0.3944548980319745</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="2">
-        <v>23399</v>
+        <v>23173</v>
       </c>
       <c r="C30" s="2">
-        <v>23409</v>
+        <v>23281</v>
       </c>
       <c r="D30">
-        <v>228.5457</v>
+        <v>1707.1654</v>
       </c>
       <c r="E30" s="3">
-        <v>11</v>
+        <v>109</v>
       </c>
       <c r="F30">
-        <v>0.3922263269972214</v>
+        <v>0.9826840921901179</v>
       </c>
       <c r="G30">
-        <v>0.4351800250019531</v>
+        <v>0.9610430158618556</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B31" s="2">
-        <v>24893</v>
+        <v>23399</v>
       </c>
       <c r="C31" s="2">
-        <v>24908</v>
+        <v>23409</v>
       </c>
       <c r="D31">
-        <v>449.3761</v>
+        <v>228.5457</v>
       </c>
       <c r="E31" s="3">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F31">
-        <v>0.6376101057567258</v>
+        <v>0.3959343508130627</v>
       </c>
       <c r="G31">
-        <v>0.6052850675143409</v>
+        <v>0.5346370607754438</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="2">
-        <v>24990</v>
+        <v>24893</v>
       </c>
       <c r="C32" s="2">
-        <v>24995</v>
+        <v>24908</v>
       </c>
       <c r="D32">
-        <v>32.39729999999999</v>
+        <v>449.3761</v>
       </c>
       <c r="E32" s="3">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F32">
-        <v>0.03792664550893772</v>
+        <v>0.6446203633925311</v>
       </c>
       <c r="G32">
-        <v>0.1092833121157502</v>
+        <v>0.7037741144752745</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="2">
-        <v>25017</v>
+        <v>24990</v>
       </c>
       <c r="C33" s="2">
-        <v>25025</v>
+        <v>24995</v>
       </c>
       <c r="D33">
-        <v>76.91200000000001</v>
+        <v>32.39729999999999</v>
       </c>
       <c r="E33" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F33">
-        <v>0.1331568761738794</v>
+        <v>0.03233486307195499</v>
       </c>
       <c r="G33">
-        <v>0.2259565495468774</v>
+        <v>0.1487871533882759</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B34" s="2">
-        <v>25050</v>
+        <v>25017</v>
       </c>
       <c r="C34" s="2">
-        <v>25138</v>
+        <v>25025</v>
       </c>
       <c r="D34">
-        <v>927.2982999999996</v>
+        <v>76.91200000000001</v>
       </c>
       <c r="E34" s="3">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="F34">
-        <v>0.8816496093164389</v>
+        <v>0.1304730233462015</v>
       </c>
       <c r="G34">
-        <v>0.796586513085395</v>
+        <v>0.3001403048472961</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B35" s="2">
-        <v>25167</v>
+        <v>25050</v>
       </c>
       <c r="C35" s="2">
-        <v>25194</v>
+        <v>25138</v>
       </c>
       <c r="D35">
-        <v>280.9065999999999</v>
+        <v>908.3814999999996</v>
       </c>
       <c r="E35" s="3">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="F35">
-        <v>0.4623554038418851</v>
+        <v>0.8820185375218204</v>
       </c>
       <c r="G35">
-        <v>0.4843069914716994</v>
+        <v>0.8663269322577586</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B36" s="2">
-        <v>26254</v>
+        <v>25167</v>
       </c>
       <c r="C36" s="2">
-        <v>26284</v>
+        <v>25194</v>
       </c>
       <c r="D36">
-        <v>206.3999999999999</v>
+        <v>280.9065999999999</v>
       </c>
       <c r="E36" s="3">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F36">
-        <v>0.3598788390323559</v>
+        <v>0.4673325094602544</v>
       </c>
       <c r="G36">
-        <v>0.4119950680153623</v>
+        <v>0.5853433600845532</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B37" s="2">
-        <v>27318</v>
+        <v>26254</v>
       </c>
       <c r="C37" s="2">
-        <v>27327</v>
+        <v>26284</v>
       </c>
       <c r="D37">
-        <v>221.052</v>
+        <v>206.3999999999999</v>
       </c>
       <c r="E37" s="3">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F37">
-        <v>0.3814677596285003</v>
+        <v>0.3629277724943648</v>
       </c>
       <c r="G37">
-        <v>0.4275146812100293</v>
+        <v>0.510179126133073</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B38" s="2">
-        <v>28536</v>
+        <v>27318</v>
       </c>
       <c r="C38" s="2">
-        <v>28551</v>
+        <v>27327</v>
       </c>
       <c r="D38">
-        <v>206.9379999999999</v>
+        <v>212.602</v>
       </c>
       <c r="E38" s="3">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F38">
-        <v>0.3606847209203766</v>
+        <v>0.3723491121467837</v>
       </c>
       <c r="G38">
-        <v>0.4125779774921692</v>
+        <v>0.5172379668846484</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B39" s="2">
-        <v>28594</v>
+        <v>28536</v>
       </c>
       <c r="C39" s="2">
-        <v>28649</v>
+        <v>28551</v>
       </c>
       <c r="D39">
-        <v>417.0256</v>
+        <v>206.9379999999999</v>
       </c>
       <c r="E39" s="3">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="F39">
-        <v>0.6090926865814696</v>
+        <v>0.3637506094791428</v>
       </c>
       <c r="G39">
-        <v>0.5854072843088688</v>
+        <v>0.510798247588736</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B40" s="2">
-        <v>28681</v>
+        <v>28594</v>
       </c>
       <c r="C40" s="2">
-        <v>28686</v>
+        <v>28649</v>
       </c>
       <c r="D40">
-        <v>21.61189999999998</v>
+        <v>417.0256</v>
       </c>
       <c r="E40" s="3">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="F40">
-        <v>0.01332068288816021</v>
+        <v>0.6159005326374197</v>
       </c>
       <c r="G40">
-        <v>0.06012128747445227</v>
+        <v>0.6849537771807839</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B41" s="2">
-        <v>28876</v>
+        <v>28681</v>
       </c>
       <c r="C41" s="2">
-        <v>28962</v>
+        <v>28686</v>
       </c>
       <c r="D41">
-        <v>1618.9602</v>
+        <v>21.61189999999998</v>
       </c>
       <c r="E41" s="3">
-        <v>87</v>
+        <v>6</v>
       </c>
       <c r="F41">
-        <v>0.9765680652594908</v>
+        <v>0.006935480698701546</v>
       </c>
       <c r="G41">
-        <v>0.9141825554339033</v>
+        <v>0.06904941484713564</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B42" s="2">
-        <v>29980</v>
+        <v>28876</v>
       </c>
       <c r="C42" s="2">
-        <v>29986</v>
+        <v>28962</v>
       </c>
       <c r="D42">
-        <v>115.9649999999999</v>
+        <v>1618.9602</v>
       </c>
       <c r="E42" s="3">
-        <v>7</v>
+        <v>87</v>
       </c>
       <c r="F42">
-        <v>0.2089081387019086</v>
+        <v>0.9785972564190827</v>
       </c>
       <c r="G42">
-        <v>0.2950947629069823</v>
+        <v>0.9555788636323356</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B43" s="2">
-        <v>30732</v>
+        <v>29980</v>
       </c>
       <c r="C43" s="2">
-        <v>30743</v>
+        <v>29986</v>
       </c>
       <c r="D43">
-        <v>71.96299999999999</v>
+        <v>115.9649999999999</v>
       </c>
       <c r="E43" s="3">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F43">
-        <v>0.1230532514725127</v>
+        <v>0.2083390940188587</v>
       </c>
       <c r="G43">
-        <v>0.2157433163904942</v>
+        <v>0.3813607307987391</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B44" s="2">
-        <v>31078</v>
+        <v>30732</v>
       </c>
       <c r="C44" s="2">
-        <v>31085</v>
+        <v>30743</v>
       </c>
       <c r="D44">
-        <v>36.72899999999994</v>
+        <v>71.96299999999999</v>
       </c>
       <c r="E44" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F44">
-        <v>0.04763546418634531</v>
+        <v>0.1200736257837337</v>
       </c>
       <c r="G44">
-        <v>0.1245486713118373</v>
+        <v>0.2877446352867636</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B45" s="2">
-        <v>31276</v>
+        <v>31078</v>
       </c>
       <c r="C45" s="2">
-        <v>31291</v>
+        <v>31085</v>
       </c>
       <c r="D45">
-        <v>146.7185999999999</v>
+        <v>36.72899999999994</v>
       </c>
       <c r="E45" s="3">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F45">
-        <v>0.2638723832477855</v>
+        <v>0.04235213061894908</v>
       </c>
       <c r="G45">
-        <v>0.3398668408302253</v>
+        <v>0.1702939387087302</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B46" s="2">
-        <v>31316</v>
+        <v>31276</v>
       </c>
       <c r="C46" s="2">
-        <v>31429</v>
+        <v>31291</v>
       </c>
       <c r="D46">
-        <v>3114.383299999999</v>
+        <v>148.5185999999999</v>
       </c>
       <c r="E46" s="3">
-        <v>114</v>
+        <v>16</v>
       </c>
       <c r="F46">
-        <v>0.9992935367647581</v>
+        <v>0.2678903362855715</v>
       </c>
       <c r="G46">
-        <v>0.9847982418885202</v>
+        <v>0.4345332776610734</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B47" s="2">
-        <v>31628</v>
+        <v>31316</v>
       </c>
       <c r="C47" s="2">
-        <v>31637</v>
+        <v>31429</v>
       </c>
       <c r="D47">
-        <v>54.21659999999999</v>
+        <v>3096.133299999999</v>
       </c>
       <c r="E47" s="3">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="F47">
-        <v>0.08584506668744148</v>
+        <v>0.9993843416042409</v>
       </c>
       <c r="G47">
-        <v>0.174931433446384</v>
+        <v>0.9946629956092238</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B48" s="2">
-        <v>31860</v>
+        <v>31628</v>
       </c>
       <c r="C48" s="2">
-        <v>31868</v>
+        <v>31637</v>
       </c>
       <c r="D48">
-        <v>30.21599999999999</v>
+        <v>54.21659999999999</v>
       </c>
       <c r="E48" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F48">
-        <v>0.03300020079329705</v>
+        <v>0.08174966912754421</v>
       </c>
       <c r="G48">
-        <v>0.1009129834566402</v>
+        <v>0.2369239425721376</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B49" s="2">
-        <v>32149</v>
+        <v>31860</v>
       </c>
       <c r="C49" s="2">
-        <v>32156</v>
+        <v>31868</v>
       </c>
       <c r="D49">
-        <v>149.3961</v>
+        <v>30.21599999999999</v>
       </c>
       <c r="E49" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F49">
-        <v>0.2684730668116977</v>
+        <v>0.0272509006209394</v>
       </c>
       <c r="G49">
-        <v>0.3434741521755378</v>
+        <v>0.1365977647882361</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B50" s="2">
-        <v>32230</v>
+        <v>32149</v>
       </c>
       <c r="C50" s="2">
-        <v>32237</v>
+        <v>32156</v>
       </c>
       <c r="D50">
-        <v>70.05099999999996</v>
+        <v>149.3961</v>
       </c>
       <c r="E50" s="3">
         <v>8</v>
       </c>
       <c r="F50">
-        <v>0.119118347841074</v>
+        <v>0.2694319979413231</v>
       </c>
       <c r="G50">
-        <v>0.21167986048754</v>
+        <v>0.4358389751055225</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B51" s="2">
-        <v>32393</v>
+        <v>32230</v>
       </c>
       <c r="C51" s="2">
-        <v>32402</v>
+        <v>32237</v>
       </c>
       <c r="D51">
-        <v>50.43609999999994</v>
+        <v>70.05099999999996</v>
       </c>
       <c r="E51" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F51">
-        <v>0.07771688975634085</v>
+        <v>0.1160226889767841</v>
       </c>
       <c r="G51">
-        <v>0.165138393174261</v>
+        <v>0.2827800209852432</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B52" s="2">
-        <v>32472</v>
+        <v>32392</v>
       </c>
       <c r="C52" s="2">
-        <v>32496</v>
+        <v>32402</v>
       </c>
       <c r="D52">
-        <v>395.6708</v>
+        <v>52.03929999999994</v>
       </c>
       <c r="E52" s="3">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F52">
-        <v>0.5890492117346623</v>
+        <v>0.07693419428810643</v>
       </c>
       <c r="G52">
-        <v>0.5715332374061791</v>
+        <v>0.229788005894911</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B53" s="2">
-        <v>33254</v>
+        <v>32472</v>
       </c>
       <c r="C53" s="2">
-        <v>33264</v>
+        <v>32496</v>
       </c>
       <c r="D53">
-        <v>255.1968</v>
+        <v>395.6708</v>
       </c>
       <c r="E53" s="3">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F53">
-        <v>0.4289949183521968</v>
+        <v>0.5956819828599371</v>
       </c>
       <c r="G53">
-        <v>0.461092292511453</v>
+        <v>0.6716661624087845</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B54" s="2">
-        <v>33298</v>
+        <v>33254</v>
       </c>
       <c r="C54" s="2">
-        <v>33303</v>
+        <v>33264</v>
       </c>
       <c r="D54">
-        <v>30.512</v>
+        <v>255.1968</v>
       </c>
       <c r="E54" s="3">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F54">
-        <v>0.03367019038659436</v>
+        <v>0.4333966494207794</v>
       </c>
       <c r="G54">
-        <v>0.1020807082382753</v>
+        <v>0.5615702182915848</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B55" s="2">
-        <v>34619</v>
+        <v>33298</v>
       </c>
       <c r="C55" s="2">
-        <v>34626</v>
+        <v>33303</v>
       </c>
       <c r="D55">
-        <v>157.7559999999999</v>
+        <v>30.512</v>
       </c>
       <c r="E55" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F55">
-        <v>0.2826534556164326</v>
+        <v>0.02794235195962758</v>
       </c>
       <c r="G55">
-        <v>0.3544793947681888</v>
+        <v>0.1383182321490529</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B56" s="2">
-        <v>34956</v>
+        <v>34619</v>
       </c>
       <c r="C56" s="2">
-        <v>34961</v>
+        <v>34626</v>
       </c>
       <c r="D56">
-        <v>15.8848</v>
+        <v>153.136</v>
       </c>
       <c r="E56" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>0.2759662315472693</v>
       </c>
       <c r="G56">
-        <v>1.384231921899607e-10</v>
+        <v>0.4413390856627818</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B57" s="2">
-        <v>38053</v>
+        <v>34956</v>
       </c>
       <c r="C57" s="2">
-        <v>38058</v>
+        <v>34961</v>
       </c>
       <c r="D57">
-        <v>184.656</v>
+        <v>18.71480000000001</v>
       </c>
       <c r="E57" s="3">
         <v>6</v>
       </c>
       <c r="F57">
-        <v>0.3264435647010323</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>0.3875292307654203</v>
+        <v>2.64566463253627e-09</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B58" s="2">
-        <v>38399</v>
+        <v>38053</v>
       </c>
       <c r="C58" s="2">
-        <v>38433</v>
+        <v>38058</v>
       </c>
       <c r="D58">
-        <v>371.783</v>
+        <v>184.656</v>
       </c>
       <c r="E58" s="3">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="F58">
-        <v>0.5654080411851008</v>
+        <v>0.3287657418673391</v>
       </c>
       <c r="G58">
-        <v>0.5552383885254273</v>
+        <v>0.4839948512369391</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B59" s="2">
-        <v>38846</v>
+        <v>38399</v>
       </c>
       <c r="C59" s="2">
-        <v>38961</v>
+        <v>38433</v>
       </c>
       <c r="D59">
-        <v>1784.594799999999</v>
+        <v>371.783</v>
       </c>
       <c r="E59" s="3">
-        <v>116</v>
+        <v>35</v>
       </c>
       <c r="F59">
-        <v>0.9841009272926893</v>
+        <v>0.5718014870571416</v>
       </c>
       <c r="G59">
-        <v>0.929618463342568</v>
+        <v>0.655902974305608</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B60" s="2">
-        <v>39903</v>
+        <v>38846</v>
       </c>
       <c r="C60" s="2">
-        <v>39978</v>
+        <v>38961</v>
       </c>
       <c r="D60">
-        <v>477.1855999999999</v>
+        <v>1785.304799999999</v>
       </c>
       <c r="E60" s="3">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="F60">
-        <v>0.6604559120148841</v>
+        <v>0.9856476605884852</v>
       </c>
       <c r="G60">
-        <v>0.6213675377238564</v>
+        <v>0.9652949603216171</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B61" s="2">
-        <v>42998</v>
+        <v>39903</v>
       </c>
       <c r="C61" s="2">
-        <v>43007</v>
+        <v>39978</v>
       </c>
       <c r="D61">
-        <v>59.02208333333333</v>
+        <v>477.1855999999999</v>
       </c>
       <c r="E61" s="3">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="F61">
-        <v>0.09607366787684769</v>
+        <v>0.667586247680412</v>
       </c>
       <c r="G61">
-        <v>0.1867445489728367</v>
+        <v>0.7188108371943616</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="1">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B62" s="2">
+        <v>42998</v>
+      </c>
+      <c r="C62" s="2">
+        <v>43007</v>
+      </c>
+      <c r="D62">
+        <v>58.44208333333333</v>
+      </c>
+      <c r="E62" s="3">
+        <v>10</v>
+      </c>
+      <c r="F62">
+        <v>0.09102348794908463</v>
+      </c>
+      <c r="G62">
+        <v>0.2501177458392068</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="1">
+        <v>163</v>
+      </c>
+      <c r="B63" s="2">
         <v>43857</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C63" s="2">
         <v>43989</v>
       </c>
-      <c r="D62">
+      <c r="D63">
         <v>3469.4015</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E63" s="3">
         <v>133</v>
       </c>
-      <c r="F62">
-        <v>0.9996923434698294</v>
-      </c>
-      <c r="G62">
-        <v>0.989785392122957</v>
+      <c r="F63">
+        <v>0.9997488631918874</v>
+      </c>
+      <c r="G63">
+        <v>0.9968206718114339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcao fim de evento
</commit_message>
<xml_diff>
--- a/low-flow-index/dados-saida/uniao_da_vitoria.xlsx
+++ b/low-flow-index/dados-saida/uniao_da_vitoria.xlsx
@@ -437,10 +437,10 @@
         <v>29</v>
       </c>
       <c r="F2">
-        <v>0.4529604389419829</v>
+        <v>0.4535277971113451</v>
       </c>
       <c r="G2">
-        <v>0.5753401078409786</v>
+        <v>0.5734791886872768</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -460,10 +460,10 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>0.1177228730614828</v>
+        <v>0.1179129418069409</v>
       </c>
       <c r="G3">
-        <v>0.2848734791496697</v>
+        <v>0.2853087006858848</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -483,10 +483,10 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>0.04884285606111181</v>
+        <v>0.04892478570585143</v>
       </c>
       <c r="G4">
-        <v>0.1829027603585654</v>
+        <v>0.1838577298970954</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -506,10 +506,10 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>0.03955750888195161</v>
+        <v>0.03962418925596779</v>
       </c>
       <c r="G5">
-        <v>0.1645731726633032</v>
+        <v>0.1655820688594732</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -529,10 +529,10 @@
         <v>41</v>
       </c>
       <c r="F6">
-        <v>0.07770909347237369</v>
+        <v>0.07783742552582337</v>
       </c>
       <c r="G6">
-        <v>0.230950582805072</v>
+        <v>0.2317004224295548</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -552,10 +552,10 @@
         <v>25</v>
       </c>
       <c r="F7">
-        <v>0.4512234141186302</v>
+        <v>0.451789584164324</v>
       </c>
       <c r="G7">
-        <v>0.5741248761263826</v>
+        <v>0.5722734111526541</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -575,10 +575,10 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>0.001006048557626691</v>
+        <v>0.001007778286129896</v>
       </c>
       <c r="G8">
-        <v>0.02641836371270655</v>
+        <v>0.02701151003266683</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -598,10 +598,10 @@
         <v>18</v>
       </c>
       <c r="F9">
-        <v>0.5294090397474582</v>
+        <v>0.530018824508887</v>
       </c>
       <c r="G9">
-        <v>0.6276488308994788</v>
+        <v>0.6254003625127171</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -621,10 +621,10 @@
         <v>34</v>
       </c>
       <c r="F10">
-        <v>0.377918467881278</v>
+        <v>0.378426221083617</v>
       </c>
       <c r="G10">
-        <v>0.5213806288392363</v>
+        <v>0.5199529679004951</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -644,10 +644,10 @@
         <v>7</v>
       </c>
       <c r="F11">
-        <v>0.1075346739753989</v>
+        <v>0.1077093146820041</v>
       </c>
       <c r="G11">
-        <v>0.2721042111986424</v>
+        <v>0.2726205171527307</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -667,10 +667,10 @@
         <v>8</v>
       </c>
       <c r="F12">
-        <v>0.05410191626796727</v>
+        <v>0.05419241365276442</v>
       </c>
       <c r="G12">
-        <v>0.1925257988762217</v>
+        <v>0.1934466027215093</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -690,10 +690,10 @@
         <v>12</v>
       </c>
       <c r="F13">
-        <v>0.02997647482037862</v>
+        <v>0.03002725819148154</v>
       </c>
       <c r="G13">
-        <v>0.1432606226521859</v>
+        <v>0.1443114674944783</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -713,10 +713,10 @@
         <v>6</v>
       </c>
       <c r="F14">
-        <v>0.009220893268835482</v>
+        <v>0.009236681532334645</v>
       </c>
       <c r="G14">
-        <v>0.07957250513004152</v>
+        <v>0.08056955282316679</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -736,10 +736,10 @@
         <v>14</v>
       </c>
       <c r="F15">
-        <v>0.2010550213662789</v>
+        <v>0.2013634510299247</v>
       </c>
       <c r="G15">
-        <v>0.374426565246658</v>
+        <v>0.3742106071737282</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -759,10 +759,10 @@
         <v>90</v>
       </c>
       <c r="F16">
-        <v>0.9471514783503885</v>
+        <v>0.9474181079555035</v>
       </c>
       <c r="G16">
-        <v>0.9213306635642655</v>
+        <v>0.9188942448901316</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -776,16 +776,16 @@
         <v>16383</v>
       </c>
       <c r="D17">
-        <v>730.4280999999996</v>
+        <v>723.2480999999997</v>
       </c>
       <c r="E17" s="3">
         <v>47</v>
       </c>
       <c r="F17">
-        <v>0.8190860946412644</v>
+        <v>0.81647365729994</v>
       </c>
       <c r="G17">
-        <v>0.8203442147426415</v>
+        <v>0.8151226585960806</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -805,10 +805,10 @@
         <v>46</v>
       </c>
       <c r="F18">
-        <v>0.8600171293204313</v>
+        <v>0.8604897950091843</v>
       </c>
       <c r="G18">
-        <v>0.8497593115723698</v>
+        <v>0.8467974070450799</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -828,10 +828,10 @@
         <v>14</v>
       </c>
       <c r="F19">
-        <v>0.3604892821217764</v>
+        <v>0.3609808876474872</v>
       </c>
       <c r="G19">
-        <v>0.5083413410509233</v>
+        <v>0.5070214096419517</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -851,10 +851,10 @@
         <v>37</v>
       </c>
       <c r="F20">
-        <v>0.8484968805086426</v>
+        <v>0.8489879025846336</v>
       </c>
       <c r="G20">
-        <v>0.8413208553348218</v>
+        <v>0.8383361418981622</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -874,10 +874,10 @@
         <v>60</v>
       </c>
       <c r="F21">
-        <v>0.5709331452572712</v>
+        <v>0.5715572111265292</v>
       </c>
       <c r="G21">
-        <v>0.6553280378850799</v>
+        <v>0.6528939738185671</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -891,16 +891,16 @@
         <v>18915</v>
       </c>
       <c r="D22">
-        <v>1363.2869</v>
+        <v>1360.6069</v>
       </c>
       <c r="E22" s="3">
         <v>63</v>
       </c>
       <c r="F22">
-        <v>0.9604439854788251</v>
+        <v>0.9604086507376332</v>
       </c>
       <c r="G22">
-        <v>0.9346513613764266</v>
+        <v>0.9321337477489449</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -920,10 +920,10 @@
         <v>22</v>
       </c>
       <c r="F23">
-        <v>0.1929737554386703</v>
+        <v>0.1932713386849009</v>
       </c>
       <c r="G23">
-        <v>0.3666017075283696</v>
+        <v>0.3664471160611598</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -943,10 +943,10 @@
         <v>57</v>
       </c>
       <c r="F24">
-        <v>0.8592211580326078</v>
+        <v>0.859695142912881</v>
       </c>
       <c r="G24">
-        <v>0.8491715539014487</v>
+        <v>0.8462078521496383</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -966,10 +966,10 @@
         <v>26</v>
       </c>
       <c r="F25">
-        <v>0.0751800696806284</v>
+        <v>0.07530439785455131</v>
       </c>
       <c r="G25">
-        <v>0.2271351965703581</v>
+        <v>0.2279042478599306</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -989,10 +989,10 @@
         <v>19</v>
       </c>
       <c r="F26">
-        <v>0.4916745529134886</v>
+        <v>0.4922658701248102</v>
       </c>
       <c r="G26">
-        <v>0.6020925612849669</v>
+        <v>0.6000282800773625</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1012,10 +1012,10 @@
         <v>70</v>
       </c>
       <c r="F27">
-        <v>0.8903041747537608</v>
+        <v>0.8907204146539784</v>
       </c>
       <c r="G27">
-        <v>0.8727518760646145</v>
+        <v>0.8698872164845448</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1035,10 +1035,10 @@
         <v>19</v>
       </c>
       <c r="F28">
-        <v>0.1530741280505891</v>
+        <v>0.1533161423450484</v>
       </c>
       <c r="G28">
-        <v>0.3255814890873994</v>
+        <v>0.3257362617517343</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1058,10 +1058,10 @@
         <v>14</v>
       </c>
       <c r="F29">
-        <v>0.2224040040683128</v>
+        <v>0.2227404065507414</v>
       </c>
       <c r="G29">
-        <v>0.3944548980319745</v>
+        <v>0.3940791602247605</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1081,10 +1081,10 @@
         <v>109</v>
       </c>
       <c r="F30">
-        <v>0.9826840921901179</v>
+        <v>0.9828044906221561</v>
       </c>
       <c r="G30">
-        <v>0.9610430158618556</v>
+        <v>0.9593250466399729</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1104,10 +1104,10 @@
         <v>11</v>
       </c>
       <c r="F31">
-        <v>0.3959343508130627</v>
+        <v>0.3964579111565711</v>
       </c>
       <c r="G31">
-        <v>0.5346370607754438</v>
+        <v>0.5331008201872918</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1127,10 +1127,10 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>0.6446203633925311</v>
+        <v>0.6452522562276861</v>
       </c>
       <c r="G32">
-        <v>0.7037741144752745</v>
+        <v>0.7010601039367004</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1150,10 +1150,10 @@
         <v>6</v>
       </c>
       <c r="F33">
-        <v>0.03233486307195499</v>
+        <v>0.03238957470902752</v>
       </c>
       <c r="G33">
-        <v>0.1487871533882759</v>
+        <v>0.1498294540412411</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1173,10 +1173,10 @@
         <v>9</v>
       </c>
       <c r="F34">
-        <v>0.1304730233462015</v>
+        <v>0.1306821138771109</v>
       </c>
       <c r="G34">
-        <v>0.3001403048472961</v>
+        <v>0.3004740081692701</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1190,16 +1190,16 @@
         <v>25138</v>
       </c>
       <c r="D35">
-        <v>908.3814999999996</v>
+        <v>896.9914999999997</v>
       </c>
       <c r="E35" s="3">
         <v>89</v>
       </c>
       <c r="F35">
-        <v>0.8820185375218204</v>
+        <v>0.879185043365764</v>
       </c>
       <c r="G35">
-        <v>0.8663269322577586</v>
+        <v>0.8609106099723336</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1219,10 +1219,10 @@
         <v>28</v>
       </c>
       <c r="F36">
-        <v>0.4673325094602544</v>
+        <v>0.4679093310140311</v>
       </c>
       <c r="G36">
-        <v>0.5853433600845532</v>
+        <v>0.5834052931635964</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1242,10 +1242,10 @@
         <v>31</v>
       </c>
       <c r="F37">
-        <v>0.3629277724943648</v>
+        <v>0.3634216869426148</v>
       </c>
       <c r="G37">
-        <v>0.510179126133073</v>
+        <v>0.5088439645220323</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1259,16 +1259,16 @@
         <v>27327</v>
       </c>
       <c r="D38">
-        <v>212.602</v>
+        <v>205.312</v>
       </c>
       <c r="E38" s="3">
         <v>10</v>
       </c>
       <c r="F38">
-        <v>0.3723491121467837</v>
+        <v>0.3617528293075056</v>
       </c>
       <c r="G38">
-        <v>0.5172379668846484</v>
+        <v>0.5075983035407062</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1288,10 +1288,10 @@
         <v>16</v>
       </c>
       <c r="F39">
-        <v>0.3637506094791428</v>
+        <v>0.3642452994200327</v>
       </c>
       <c r="G39">
-        <v>0.510798247588736</v>
+        <v>0.5094579583081865</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1311,10 +1311,10 @@
         <v>56</v>
       </c>
       <c r="F40">
-        <v>0.6159005326374197</v>
+        <v>0.6165322311485333</v>
       </c>
       <c r="G40">
-        <v>0.6849537771807839</v>
+        <v>0.6823407821152064</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1334,10 +1334,10 @@
         <v>6</v>
       </c>
       <c r="F41">
-        <v>0.006935480698701546</v>
+        <v>0.006947369547073484</v>
       </c>
       <c r="G41">
-        <v>0.06904941484713564</v>
+        <v>0.07000207617059133</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1357,10 +1357,10 @@
         <v>87</v>
       </c>
       <c r="F42">
-        <v>0.9785972564190827</v>
+        <v>0.9787383224033448</v>
       </c>
       <c r="G42">
-        <v>0.9555788636323356</v>
+        <v>0.9537314912445886</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1380,10 +1380,10 @@
         <v>7</v>
       </c>
       <c r="F43">
-        <v>0.2083390940188587</v>
+        <v>0.2086571795210225</v>
       </c>
       <c r="G43">
-        <v>0.3813607307987391</v>
+        <v>0.3810898700999379</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1403,10 +1403,10 @@
         <v>12</v>
       </c>
       <c r="F44">
-        <v>0.1200736257837337</v>
+        <v>0.1202672255916622</v>
       </c>
       <c r="G44">
-        <v>0.2877446352867636</v>
+        <v>0.2881611314281282</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1426,10 +1426,10 @@
         <v>8</v>
       </c>
       <c r="F45">
-        <v>0.04235213061894908</v>
+        <v>0.042423416922967</v>
       </c>
       <c r="G45">
-        <v>0.1702939387087302</v>
+        <v>0.1712876586252341</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1449,10 +1449,10 @@
         <v>16</v>
       </c>
       <c r="F46">
-        <v>0.2678903362855715</v>
+        <v>0.2682829346714851</v>
       </c>
       <c r="G46">
-        <v>0.4345332776610734</v>
+        <v>0.4338290679515271</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1466,16 +1466,16 @@
         <v>31429</v>
       </c>
       <c r="D47">
-        <v>3096.133299999999</v>
+        <v>3084.823299999999</v>
       </c>
       <c r="E47" s="3">
         <v>114</v>
       </c>
       <c r="F47">
-        <v>0.9993843416042409</v>
+        <v>0.9993753498865218</v>
       </c>
       <c r="G47">
-        <v>0.9946629956092238</v>
+        <v>0.9941207240915463</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1495,10 +1495,10 @@
         <v>10</v>
       </c>
       <c r="F48">
-        <v>0.08174966912754421</v>
+        <v>0.08188437329935869</v>
       </c>
       <c r="G48">
-        <v>0.2369239425721376</v>
+        <v>0.2376428082713817</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1518,10 +1518,10 @@
         <v>9</v>
       </c>
       <c r="F49">
-        <v>0.0272509006209394</v>
+        <v>0.02729713181482321</v>
       </c>
       <c r="G49">
-        <v>0.1365977647882361</v>
+        <v>0.1376565718724659</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1541,10 +1541,10 @@
         <v>8</v>
       </c>
       <c r="F50">
-        <v>0.2694319979413231</v>
+        <v>0.2698264173423163</v>
       </c>
       <c r="G50">
-        <v>0.4358389751055225</v>
+        <v>0.4351239267940162</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1564,10 +1564,10 @@
         <v>8</v>
       </c>
       <c r="F51">
-        <v>0.1160226889767841</v>
+        <v>0.1162101971520798</v>
       </c>
       <c r="G51">
-        <v>0.2827800209852432</v>
+        <v>0.2832287843870434</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1587,10 +1587,10 @@
         <v>11</v>
       </c>
       <c r="F52">
-        <v>0.07693419428810643</v>
+        <v>0.07706130081100657</v>
       </c>
       <c r="G52">
-        <v>0.229788005894911</v>
+        <v>0.2305437474700897</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1610,10 +1610,10 @@
         <v>25</v>
       </c>
       <c r="F53">
-        <v>0.5956819828599371</v>
+        <v>0.5963113107494582</v>
       </c>
       <c r="G53">
-        <v>0.6716661624087845</v>
+        <v>0.6691306268091346</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1633,10 +1633,10 @@
         <v>11</v>
       </c>
       <c r="F54">
-        <v>0.4333966494207794</v>
+        <v>0.4339500842377791</v>
       </c>
       <c r="G54">
-        <v>0.5615702182915848</v>
+        <v>0.5598173803898702</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1656,10 +1656,10 @@
         <v>6</v>
       </c>
       <c r="F55">
-        <v>0.02794235195962758</v>
+        <v>0.02798973924320487</v>
       </c>
       <c r="G55">
-        <v>0.1383182321490529</v>
+        <v>0.1393752351845627</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1673,16 +1673,16 @@
         <v>34626</v>
       </c>
       <c r="D56">
-        <v>153.136</v>
+        <v>148.666</v>
       </c>
       <c r="E56" s="3">
         <v>8</v>
       </c>
       <c r="F56">
-        <v>0.2759662315472693</v>
+        <v>0.2685424323926916</v>
       </c>
       <c r="G56">
-        <v>0.4413390856627818</v>
+        <v>0.434046981907281</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1705,7 +1705,7 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>2.64566463253627e-09</v>
+        <v>3.120731044221785e-09</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1725,10 +1725,10 @@
         <v>6</v>
       </c>
       <c r="F58">
-        <v>0.3287657418673391</v>
+        <v>0.3292258722167992</v>
       </c>
       <c r="G58">
-        <v>0.4839948512369391</v>
+        <v>0.4828777012573838</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1748,10 +1748,10 @@
         <v>35</v>
       </c>
       <c r="F59">
-        <v>0.5718014870571416</v>
+        <v>0.5724257799799968</v>
       </c>
       <c r="G59">
-        <v>0.655902974305608</v>
+        <v>0.6534652306011058</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1771,15 +1771,15 @@
         <v>116</v>
       </c>
       <c r="F60">
-        <v>0.9856476605884852</v>
+        <v>0.9857520546122556</v>
       </c>
       <c r="G60">
-        <v>0.9652949603216171</v>
+        <v>0.9636870431529652</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B61" s="2">
         <v>39903</v>
@@ -1794,15 +1794,15 @@
         <v>76</v>
       </c>
       <c r="F61">
-        <v>0.667586247680412</v>
+        <v>0.6682154361592868</v>
       </c>
       <c r="G61">
-        <v>0.7188108371943616</v>
+        <v>0.7160242700099764</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" s="1">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B62" s="2">
         <v>42998</v>
@@ -1817,15 +1817,15 @@
         <v>10</v>
       </c>
       <c r="F62">
-        <v>0.09102348794908463</v>
+        <v>0.09117270117404355</v>
       </c>
       <c r="G62">
-        <v>0.2501177458392068</v>
+        <v>0.2507645106598095</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="1">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B63" s="2">
         <v>43857</v>
@@ -1840,10 +1840,10 @@
         <v>133</v>
       </c>
       <c r="F63">
-        <v>0.9997488631918874</v>
+        <v>0.9997524188875809</v>
       </c>
       <c r="G63">
-        <v>0.9968206718114339</v>
+        <v>0.9965156299081206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizacao uniao da vitoria 27-10
</commit_message>
<xml_diff>
--- a/low-flow-index/dados-saida/uniao_da_vitoria.xlsx
+++ b/low-flow-index/dados-saida/uniao_da_vitoria.xlsx
@@ -394,7 +394,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -437,10 +437,10 @@
         <v>29</v>
       </c>
       <c r="F2">
-        <v>0.4535277971113451</v>
+        <v>0.456438285308356</v>
       </c>
       <c r="G2">
-        <v>0.5734791886872768</v>
+        <v>0.5946080815016426</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -460,10 +460,10 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>0.1179129418069409</v>
+        <v>0.1188904404129971</v>
       </c>
       <c r="G3">
-        <v>0.2853087006858848</v>
+        <v>0.292207416994111</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -483,10 +483,10 @@
         <v>17</v>
       </c>
       <c r="F4">
-        <v>0.04892478570585143</v>
+        <v>0.04934630657270472</v>
       </c>
       <c r="G4">
-        <v>0.1838577298970954</v>
+        <v>0.1859492534638571</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -506,10 +506,10 @@
         <v>9</v>
       </c>
       <c r="F5">
-        <v>0.03962418925596779</v>
+        <v>0.03996727157481791</v>
       </c>
       <c r="G5">
-        <v>0.1655820688594732</v>
+        <v>0.1669321499764016</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -529,10 +529,10 @@
         <v>41</v>
       </c>
       <c r="F6">
-        <v>0.07783742552582337</v>
+        <v>0.07849757518135056</v>
       </c>
       <c r="G6">
-        <v>0.2317004224295548</v>
+        <v>0.2359414138669834</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -552,10 +552,10 @@
         <v>25</v>
       </c>
       <c r="F7">
-        <v>0.451789584164324</v>
+        <v>0.4546940260524142</v>
       </c>
       <c r="G7">
-        <v>0.5722734111526541</v>
+        <v>0.5933556422553211</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -575,10 +575,10 @@
         <v>6</v>
       </c>
       <c r="F8">
-        <v>0.001007778286129896</v>
+        <v>0.001016679896926618</v>
       </c>
       <c r="G8">
-        <v>0.02701151003266683</v>
+        <v>0.02568731204238746</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -598,10 +598,10 @@
         <v>18</v>
       </c>
       <c r="F9">
-        <v>0.530018824508887</v>
+        <v>0.5331444704134104</v>
       </c>
       <c r="G9">
-        <v>0.6254003625127171</v>
+        <v>0.6483240132782805</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -621,10 +621,10 @@
         <v>34</v>
       </c>
       <c r="F10">
-        <v>0.378426221083617</v>
+        <v>0.3810327115690741</v>
       </c>
       <c r="G10">
-        <v>0.5199529679004951</v>
+        <v>0.5388323385177153</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -644,10 +644,10 @@
         <v>7</v>
       </c>
       <c r="F11">
-        <v>0.1077093146820041</v>
+        <v>0.108607523417468</v>
       </c>
       <c r="G11">
-        <v>0.2726205171527307</v>
+        <v>0.2788730313709404</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -661,16 +661,16 @@
         <v>15660</v>
       </c>
       <c r="D12">
-        <v>41.86799999999998</v>
+        <v>41.64799999999998</v>
       </c>
       <c r="E12" s="3">
         <v>8</v>
       </c>
       <c r="F12">
-        <v>0.05419241365276442</v>
+        <v>0.05415296938776069</v>
       </c>
       <c r="G12">
-        <v>0.1934466027215093</v>
+        <v>0.1950169135912066</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -690,10 +690,10 @@
         <v>12</v>
       </c>
       <c r="F13">
-        <v>0.03002725819148154</v>
+        <v>0.03028856132912447</v>
       </c>
       <c r="G13">
-        <v>0.1443114674944783</v>
+        <v>0.1448698362448913</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -713,10 +713,10 @@
         <v>6</v>
       </c>
       <c r="F14">
-        <v>0.009236681532334645</v>
+        <v>0.009317928295665977</v>
       </c>
       <c r="G14">
-        <v>0.08056955282316679</v>
+        <v>0.07939398569248958</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -736,10 +736,10 @@
         <v>14</v>
       </c>
       <c r="F15">
-        <v>0.2013634510299247</v>
+        <v>0.2029488327451937</v>
       </c>
       <c r="G15">
-        <v>0.3742106071737282</v>
+        <v>0.3857813671399947</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -759,10 +759,10 @@
         <v>90</v>
       </c>
       <c r="F16">
-        <v>0.9474181079555035</v>
+        <v>0.948769130448873</v>
       </c>
       <c r="G16">
-        <v>0.9188942448901316</v>
+        <v>0.9359366468609942</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -776,16 +776,16 @@
         <v>16383</v>
       </c>
       <c r="D17">
-        <v>723.2480999999997</v>
+        <v>697.0880999999997</v>
       </c>
       <c r="E17" s="3">
         <v>47</v>
       </c>
       <c r="F17">
-        <v>0.81647365729994</v>
+        <v>0.8073484016113568</v>
       </c>
       <c r="G17">
-        <v>0.8151226585960806</v>
+        <v>0.8309037999330935</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -805,15 +805,15 @@
         <v>46</v>
       </c>
       <c r="F18">
-        <v>0.8604897950091843</v>
+        <v>0.8628971389059762</v>
       </c>
       <c r="G18">
-        <v>0.8467974070450799</v>
+        <v>0.869406435400824</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2">
         <v>17893</v>
@@ -828,15 +828,15 @@
         <v>14</v>
       </c>
       <c r="F19">
-        <v>0.3609808876474872</v>
+        <v>0.3635048544208712</v>
       </c>
       <c r="G19">
-        <v>0.5070214096419517</v>
+        <v>0.5253095515545443</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2">
         <v>17926</v>
@@ -851,15 +851,15 @@
         <v>37</v>
       </c>
       <c r="F20">
-        <v>0.8489879025846336</v>
+        <v>0.8514897811709355</v>
       </c>
       <c r="G20">
-        <v>0.8383361418981622</v>
+        <v>0.8613344367964542</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2">
         <v>18201</v>
@@ -868,21 +868,21 @@
         <v>18260</v>
       </c>
       <c r="D21">
-        <v>370.9396999999999</v>
+        <v>370.7196999999999</v>
       </c>
       <c r="E21" s="3">
         <v>60</v>
       </c>
       <c r="F21">
-        <v>0.5715572111265292</v>
+        <v>0.5745273194679344</v>
       </c>
       <c r="G21">
-        <v>0.6528939738185671</v>
+        <v>0.6764188183050507</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2">
         <v>18853</v>
@@ -891,21 +891,21 @@
         <v>18915</v>
       </c>
       <c r="D22">
-        <v>1360.6069</v>
+        <v>1352.8269</v>
       </c>
       <c r="E22" s="3">
         <v>63</v>
       </c>
       <c r="F22">
-        <v>0.9604086507376332</v>
+        <v>0.9607888661344086</v>
       </c>
       <c r="G22">
-        <v>0.9321337477489449</v>
+        <v>0.9468712271283568</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2">
         <v>19050</v>
@@ -920,15 +920,15 @@
         <v>22</v>
       </c>
       <c r="F23">
-        <v>0.1932713386849009</v>
+        <v>0.1948010493038771</v>
       </c>
       <c r="G23">
-        <v>0.3664471160611598</v>
+        <v>0.3776063161124989</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" s="2">
         <v>19093</v>
@@ -943,15 +943,15 @@
         <v>57</v>
       </c>
       <c r="F24">
-        <v>0.859695142912881</v>
+        <v>0.8621092778049834</v>
       </c>
       <c r="G24">
-        <v>0.8462078521496383</v>
+        <v>0.8688454646257577</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" s="2">
         <v>20119</v>
@@ -966,15 +966,15 @@
         <v>26</v>
       </c>
       <c r="F25">
-        <v>0.07530439785455131</v>
+        <v>0.07594396051253505</v>
       </c>
       <c r="G25">
-        <v>0.2279042478599306</v>
+        <v>0.23196556401993</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="2">
         <v>20778</v>
@@ -989,15 +989,15 @@
         <v>19</v>
       </c>
       <c r="F26">
-        <v>0.4922658701248102</v>
+        <v>0.495298089818908</v>
       </c>
       <c r="G26">
-        <v>0.6000282800773625</v>
+        <v>0.6221299527131881</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2">
         <v>21855</v>
@@ -1006,21 +1006,21 @@
         <v>21924</v>
       </c>
       <c r="D27">
-        <v>938.6927999999998</v>
+        <v>938.4727999999998</v>
       </c>
       <c r="E27" s="3">
         <v>70</v>
       </c>
       <c r="F27">
-        <v>0.8907204146539784</v>
+        <v>0.8927804017850125</v>
       </c>
       <c r="G27">
-        <v>0.8698872164845448</v>
+        <v>0.8911477512829834</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="2">
         <v>21941</v>
@@ -1035,15 +1035,15 @@
         <v>19</v>
       </c>
       <c r="F28">
-        <v>0.1533161423450484</v>
+        <v>0.1545605211018792</v>
       </c>
       <c r="G28">
-        <v>0.3257362617517343</v>
+        <v>0.3347399160960936</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="2">
         <v>23008</v>
@@ -1058,15 +1058,15 @@
         <v>14</v>
       </c>
       <c r="F29">
-        <v>0.2227404065507414</v>
+        <v>0.2244693258856998</v>
       </c>
       <c r="G29">
-        <v>0.3940791602247605</v>
+        <v>0.4067000445763652</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="1">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="2">
         <v>23173</v>
@@ -1081,15 +1081,15 @@
         <v>109</v>
       </c>
       <c r="F30">
-        <v>0.9828044906221561</v>
+        <v>0.9834109810777103</v>
       </c>
       <c r="G30">
-        <v>0.9593250466399729</v>
+        <v>0.9705449141039382</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="1">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="2">
         <v>23399</v>
@@ -1104,15 +1104,15 @@
         <v>11</v>
       </c>
       <c r="F31">
-        <v>0.3964579111565711</v>
+        <v>0.3991451284445828</v>
       </c>
       <c r="G31">
-        <v>0.5331008201872918</v>
+        <v>0.5525639154786957</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="1">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2">
         <v>24893</v>
@@ -1127,15 +1127,15 @@
         <v>16</v>
       </c>
       <c r="F32">
-        <v>0.6452522562276861</v>
+        <v>0.6484864247347032</v>
       </c>
       <c r="G32">
-        <v>0.7010601039367004</v>
+        <v>0.7256515131078404</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" s="2">
         <v>24990</v>
@@ -1150,15 +1150,15 @@
         <v>6</v>
       </c>
       <c r="F33">
-        <v>0.03238957470902752</v>
+        <v>0.03267108690801651</v>
       </c>
       <c r="G33">
-        <v>0.1498294540412411</v>
+        <v>0.1505850884739003</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="2">
         <v>25017</v>
@@ -1173,38 +1173,38 @@
         <v>9</v>
       </c>
       <c r="F34">
-        <v>0.1306821138771109</v>
+        <v>0.1317573562949799</v>
       </c>
       <c r="G34">
-        <v>0.3004740081692701</v>
+        <v>0.3081553789870479</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2">
         <v>25050</v>
       </c>
       <c r="C35" s="2">
-        <v>25138</v>
+        <v>25137</v>
       </c>
       <c r="D35">
-        <v>896.9914999999997</v>
+        <v>870.3554999999998</v>
       </c>
       <c r="E35" s="3">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F35">
-        <v>0.879185043365764</v>
+        <v>0.8734995432028833</v>
       </c>
       <c r="G35">
-        <v>0.8609106099723336</v>
+        <v>0.8770109888807145</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" s="2">
         <v>25167</v>
@@ -1219,15 +1219,15 @@
         <v>28</v>
       </c>
       <c r="F36">
-        <v>0.4679093310140311</v>
+        <v>0.4708679492544749</v>
       </c>
       <c r="G36">
-        <v>0.5834052931635964</v>
+        <v>0.6049103722871053</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B37" s="2">
         <v>26254</v>
@@ -1242,15 +1242,15 @@
         <v>31</v>
       </c>
       <c r="F37">
-        <v>0.3634216869426148</v>
+        <v>0.365957456839671</v>
       </c>
       <c r="G37">
-        <v>0.5088439645220323</v>
+        <v>0.5272164035966458</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" s="1">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="2">
         <v>27318</v>
@@ -1259,21 +1259,21 @@
         <v>27327</v>
       </c>
       <c r="D38">
-        <v>205.312</v>
+        <v>193.402</v>
       </c>
       <c r="E38" s="3">
         <v>10</v>
       </c>
       <c r="F38">
-        <v>0.3617528293075056</v>
+        <v>0.3456312613568117</v>
       </c>
       <c r="G38">
-        <v>0.5075983035407062</v>
+        <v>0.5112601163553028</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B39" s="2">
         <v>28536</v>
@@ -1288,15 +1288,15 @@
         <v>16</v>
       </c>
       <c r="F39">
-        <v>0.3642452994200327</v>
+        <v>0.366785033373981</v>
       </c>
       <c r="G39">
-        <v>0.5094579583081865</v>
+        <v>0.5278587260426937</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B40" s="2">
         <v>28594</v>
@@ -1311,15 +1311,15 @@
         <v>56</v>
       </c>
       <c r="F40">
-        <v>0.6165322311485333</v>
+        <v>0.6197667320535365</v>
       </c>
       <c r="G40">
-        <v>0.6823407821152064</v>
+        <v>0.706644830267916</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="A41" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B41" s="2">
         <v>28681</v>
@@ -1334,15 +1334,15 @@
         <v>6</v>
       </c>
       <c r="F41">
-        <v>0.006947369547073484</v>
+        <v>0.007008550576576805</v>
       </c>
       <c r="G41">
-        <v>0.07000207617059133</v>
+        <v>0.06866786639844855</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42" s="2">
         <v>28876</v>
@@ -1357,15 +1357,15 @@
         <v>87</v>
       </c>
       <c r="F42">
-        <v>0.9787383224033448</v>
+        <v>0.9794497154816091</v>
       </c>
       <c r="G42">
-        <v>0.9537314912445886</v>
+        <v>0.9659376638389008</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43" s="2">
         <v>29980</v>
@@ -1380,15 +1380,15 @@
         <v>7</v>
       </c>
       <c r="F43">
-        <v>0.2086571795210225</v>
+        <v>0.2102921147728999</v>
       </c>
       <c r="G43">
-        <v>0.3810898700999379</v>
+        <v>0.3930248707346073</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="1">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B44" s="2">
         <v>30732</v>
@@ -1403,15 +1403,15 @@
         <v>12</v>
       </c>
       <c r="F44">
-        <v>0.1202672255916622</v>
+        <v>0.1212628699479383</v>
       </c>
       <c r="G44">
-        <v>0.2881611314281282</v>
+        <v>0.295206266264294</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B45" s="2">
         <v>31078</v>
@@ -1426,15 +1426,15 @@
         <v>8</v>
       </c>
       <c r="F45">
-        <v>0.042423416922967</v>
+        <v>0.04279019191667693</v>
       </c>
       <c r="G45">
-        <v>0.1712876586252341</v>
+        <v>0.1728636118895857</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="1">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B46" s="2">
         <v>31276</v>
@@ -1449,15 +1449,15 @@
         <v>16</v>
       </c>
       <c r="F46">
-        <v>0.2682829346714851</v>
+        <v>0.2703000266792889</v>
       </c>
       <c r="G46">
-        <v>0.4338290679515271</v>
+        <v>0.4485209877096592</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="1">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" s="2">
         <v>31316</v>
@@ -1466,21 +1466,21 @@
         <v>31429</v>
       </c>
       <c r="D47">
-        <v>3084.823299999999</v>
+        <v>3052.843299999999</v>
       </c>
       <c r="E47" s="3">
         <v>114</v>
       </c>
       <c r="F47">
-        <v>0.9993753498865218</v>
+        <v>0.9993675357725381</v>
       </c>
       <c r="G47">
-        <v>0.9941207240915463</v>
+        <v>0.9965394875327398</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B48" s="2">
         <v>31628</v>
@@ -1495,15 +1495,15 @@
         <v>10</v>
       </c>
       <c r="F48">
-        <v>0.08188437329935869</v>
+        <v>0.0825772855254862</v>
       </c>
       <c r="G48">
-        <v>0.2376428082713817</v>
+        <v>0.2421677103570429</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" s="2">
         <v>31860</v>
@@ -1518,15 +1518,15 @@
         <v>9</v>
       </c>
       <c r="F49">
-        <v>0.02729713181482321</v>
+        <v>0.02753501549482289</v>
       </c>
       <c r="G49">
-        <v>0.1376565718724659</v>
+        <v>0.1379852508818057</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" s="2">
         <v>32149</v>
@@ -1541,15 +1541,15 @@
         <v>8</v>
       </c>
       <c r="F50">
-        <v>0.2698264173423163</v>
+        <v>0.2718528427878296</v>
       </c>
       <c r="G50">
-        <v>0.4351239267940162</v>
+        <v>0.4498823105983869</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" s="2">
         <v>32230</v>
@@ -1564,15 +1564,15 @@
         <v>8</v>
       </c>
       <c r="F51">
-        <v>0.1162101971520798</v>
+        <v>0.1171745368948168</v>
       </c>
       <c r="G51">
-        <v>0.2832287843870434</v>
+        <v>0.2900209881439849</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B52" s="2">
         <v>32392</v>
@@ -1587,15 +1587,15 @@
         <v>11</v>
       </c>
       <c r="F52">
-        <v>0.07706130081100657</v>
+        <v>0.07771514914858633</v>
       </c>
       <c r="G52">
-        <v>0.2305437474700897</v>
+        <v>0.2347298494939028</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B53" s="2">
         <v>32472</v>
@@ -1610,15 +1610,15 @@
         <v>25</v>
       </c>
       <c r="F53">
-        <v>0.5963113107494582</v>
+        <v>0.5995345463383216</v>
       </c>
       <c r="G53">
-        <v>0.6691306268091346</v>
+        <v>0.6931786664959569</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="1">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B54" s="2">
         <v>33254</v>
@@ -1633,15 +1633,15 @@
         <v>11</v>
       </c>
       <c r="F54">
-        <v>0.4339500842377791</v>
+        <v>0.4367896741435222</v>
       </c>
       <c r="G54">
-        <v>0.5598173803898702</v>
+        <v>0.5804058927496979</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="1">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B55" s="2">
         <v>33298</v>
@@ -1656,38 +1656,38 @@
         <v>6</v>
       </c>
       <c r="F55">
-        <v>0.02798973924320487</v>
+        <v>0.02823357069298679</v>
       </c>
       <c r="G55">
-        <v>0.1393752351845627</v>
+        <v>0.1397623444467889</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="1">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B56" s="2">
-        <v>34619</v>
+        <v>34620</v>
       </c>
       <c r="C56" s="2">
         <v>34626</v>
       </c>
       <c r="D56">
-        <v>148.666</v>
+        <v>139.9039999999999</v>
       </c>
       <c r="E56" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56">
-        <v>0.2685424323926916</v>
+        <v>0.2548787708821944</v>
       </c>
       <c r="G56">
-        <v>0.434046981907281</v>
+        <v>0.4348164264292126</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="1">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B57" s="2">
         <v>34956</v>
@@ -1705,12 +1705,12 @@
         <v>0</v>
       </c>
       <c r="G57">
-        <v>3.120731044221785e-09</v>
+        <v>1.759430566470838e-09</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" s="1">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B58" s="2">
         <v>38053</v>
@@ -1725,15 +1725,15 @@
         <v>6</v>
       </c>
       <c r="F58">
-        <v>0.3292258722167992</v>
+        <v>0.3315888457356055</v>
       </c>
       <c r="G58">
-        <v>0.4828777012573838</v>
+        <v>0.5000217193025353</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B59" s="2">
         <v>38399</v>
@@ -1748,15 +1748,15 @@
         <v>35</v>
       </c>
       <c r="F59">
-        <v>0.5724257799799968</v>
+        <v>0.5756241970409621</v>
       </c>
       <c r="G59">
-        <v>0.6534652306011058</v>
+        <v>0.6771570090182866</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B60" s="2">
         <v>38846</v>
@@ -1771,15 +1771,15 @@
         <v>116</v>
       </c>
       <c r="F60">
-        <v>0.9857520546122556</v>
+        <v>0.9862774060705517</v>
       </c>
       <c r="G60">
-        <v>0.9636870431529652</v>
+        <v>0.9740845997455293</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" s="2">
         <v>39903</v>
@@ -1794,10 +1794,10 @@
         <v>76</v>
       </c>
       <c r="F61">
-        <v>0.6682154361592868</v>
+        <v>0.671434627507651</v>
       </c>
       <c r="G61">
-        <v>0.7160242700099764</v>
+        <v>0.7407765438013726</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1817,10 +1817,10 @@
         <v>10</v>
       </c>
       <c r="F62">
-        <v>0.09117270117404355</v>
+        <v>0.09194020613779094</v>
       </c>
       <c r="G62">
-        <v>0.2507645106598095</v>
+        <v>0.255926962991087</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1840,10 +1840,33 @@
         <v>133</v>
       </c>
       <c r="F63">
-        <v>0.9997524188875809</v>
+        <v>0.9997699366975298</v>
       </c>
       <c r="G63">
-        <v>0.9965156299081206</v>
+        <v>0.9981836187804234</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="1">
+        <v>164</v>
+      </c>
+      <c r="B64" s="2">
+        <v>44123</v>
+      </c>
+      <c r="C64" s="2">
+        <v>44130</v>
+      </c>
+      <c r="D64">
+        <v>318.822396</v>
+      </c>
+      <c r="E64" s="3">
+        <v>8</v>
+      </c>
+      <c r="F64">
+        <v>0.5173987797657653</v>
+      </c>
+      <c r="G64">
+        <v>0.6374912600607676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>